<commit_message>
refreshing on VBA. Need to figure out how to allow user to select multiple choices on the dropdown.
</commit_message>
<xml_diff>
--- a/Budget Planner.xlsx
+++ b/Budget Planner.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Planner" sheetId="3" r:id="rId1"/>
     <sheet name="Budget" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Actual Cost</t>
   </si>
@@ -69,12 +64,6 @@
     <t>Entertainment</t>
   </si>
   <si>
-    <t>Banking/Debit/Billing</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
     <t>Utilities/Rent</t>
   </si>
   <si>
@@ -88,13 +77,61 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Rent/Mortgage</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Online Shopping</t>
+  </si>
+  <si>
+    <t>Loan/Bills</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food </t>
+  </si>
+  <si>
+    <t>Drinks</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Food/Entertainment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +147,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,10 +187,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,7 +468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:F17"/>
+  <dimension ref="A8:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
@@ -427,20 +488,25 @@
   </cols>
   <sheetData>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -448,55 +514,158 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transport" sqref="C13">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transport" sqref="C14">
       <formula1>$A$13:$A$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Utilities/Rent" sqref="D14">
+      <formula1>$A$19:$A$23</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Shopping" sqref="E14">
+      <formula1>$A$25:$A$27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Food/Entertainment" sqref="C17">
+      <formula1>$A$33:$A$37</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Loan/Bills" sqref="D17">
+      <formula1>$A$29:$A$31</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8 D10">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>